<commit_message>
improted JSON type test case from Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase_v1.xlsx
+++ b/src/test/resources/TestCase_v1.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaa./Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77A37AE3-0412-AF47-843E-E56FBC29B283}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445ACB78-768A-5141-B8A0-CE5359A44DD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="720" windowWidth="27840" windowHeight="17040" xr2:uid="{EAF4D39D-FDAF-E24F-BE2E-C615BF7C31AC}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterTestCaseSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="RegisterTestCaseSheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
   <si>
     <t>CaseId</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>pwd</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"13344445555","pwd":"123456"}</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"13344445555","pwd":""}</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"","pwd":"123456"}</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"1334444","pwd":"123456"}</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"13344445555","pwd":"12345"}</t>
+  </si>
+  <si>
+    <t>{"mobilephone":"13344445545","pwd":"123456"}</t>
   </si>
 </sst>
 </file>
@@ -449,7 +470,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,7 +609,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="1">
-        <v>13344445555</v>
+        <v>13344445355</v>
       </c>
       <c r="G6" s="1">
         <v>123456</v>
@@ -628,12 +649,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FB5862-C2D4-9C4B-9F52-95B3F6A7902F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="63.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3:C7" r:id="rId1" display="http://47.107.166.132:8080/futureloan/mvc/api/member/register" xr:uid="{4DFFEFA4-2CA4-E842-AED4-8D3C55813086}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{C8C0C03F-B6AB-CF48-B5B5-95B844F17D41}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>